<commit_message>
Add importOffers and importCompanies endpoints
</commit_message>
<xml_diff>
--- a/files/input/productsDataMDB.xlsx
+++ b/files/input/productsDataMDB.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="43">
   <si>
     <t>DB</t>
   </si>
@@ -94,6 +94,60 @@
   </si>
   <si>
     <t>startingPriceTotal</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>65489621</t>
+  </si>
+  <si>
+    <t>68546513</t>
+  </si>
+  <si>
+    <t>68546511</t>
   </si>
 </sst>
 </file>
@@ -129,8 +183,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -414,11 +471,12 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
@@ -426,7 +484,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B1" t="s">
@@ -435,7 +493,7 @@
       <c r="C1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E1" t="s">
@@ -464,8 +522,8 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -473,8 +531,8 @@
       <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="D2">
-        <v>65489621</v>
+      <c r="D2" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
@@ -502,8 +560,8 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
+      <c r="A3" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -511,8 +569,8 @@
       <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="D3">
-        <v>68546513</v>
+      <c r="D3" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
@@ -540,8 +598,8 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
+      <c r="A4" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -549,8 +607,8 @@
       <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="D4">
-        <v>68546511</v>
+      <c r="D4" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
@@ -578,8 +636,8 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
+      <c r="A5" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -587,8 +645,8 @@
       <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="D5">
-        <v>65489621</v>
+      <c r="D5" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="E5" t="s">
         <v>0</v>
@@ -616,8 +674,8 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
+      <c r="A6" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -625,8 +683,8 @@
       <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="D6">
-        <v>68546513</v>
+      <c r="D6" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="E6" t="s">
         <v>0</v>
@@ -654,8 +712,8 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
+      <c r="A7" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -663,8 +721,8 @@
       <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="D7">
-        <v>68546511</v>
+      <c r="D7" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="E7" t="s">
         <v>1</v>
@@ -692,8 +750,8 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
+      <c r="A8" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
@@ -701,8 +759,8 @@
       <c r="C8" t="s">
         <v>14</v>
       </c>
-      <c r="D8">
-        <v>65489621</v>
+      <c r="D8" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="E8" t="s">
         <v>0</v>
@@ -730,8 +788,8 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
+      <c r="A9" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
@@ -739,8 +797,8 @@
       <c r="C9" t="s">
         <v>15</v>
       </c>
-      <c r="D9">
-        <v>68546513</v>
+      <c r="D9" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="E9" t="s">
         <v>0</v>
@@ -768,8 +826,8 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
+      <c r="A10" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
@@ -777,8 +835,8 @@
       <c r="C10" t="s">
         <v>16</v>
       </c>
-      <c r="D10">
-        <v>68546511</v>
+      <c r="D10" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="E10" t="s">
         <v>1</v>
@@ -806,8 +864,8 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
+      <c r="A11" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
@@ -815,8 +873,8 @@
       <c r="C11" t="s">
         <v>14</v>
       </c>
-      <c r="D11">
-        <v>65489621</v>
+      <c r="D11" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="E11" t="s">
         <v>0</v>
@@ -844,8 +902,8 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
+      <c r="A12" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
@@ -853,8 +911,8 @@
       <c r="C12" t="s">
         <v>15</v>
       </c>
-      <c r="D12">
-        <v>68546513</v>
+      <c r="D12" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="E12" t="s">
         <v>0</v>
@@ -882,8 +940,8 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
+      <c r="A13" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="B13" t="s">
         <v>4</v>
@@ -891,8 +949,8 @@
       <c r="C13" t="s">
         <v>16</v>
       </c>
-      <c r="D13">
-        <v>68546511</v>
+      <c r="D13" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="E13" t="s">
         <v>1</v>
@@ -920,8 +978,8 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
+      <c r="A14" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
@@ -929,8 +987,8 @@
       <c r="C14" t="s">
         <v>14</v>
       </c>
-      <c r="D14">
-        <v>65489621</v>
+      <c r="D14" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="E14" t="s">
         <v>0</v>
@@ -958,8 +1016,8 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
+      <c r="A15" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="B15" t="s">
         <v>3</v>
@@ -967,8 +1025,8 @@
       <c r="C15" t="s">
         <v>15</v>
       </c>
-      <c r="D15">
-        <v>68546513</v>
+      <c r="D15" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="E15" t="s">
         <v>0</v>
@@ -996,8 +1054,8 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
+      <c r="A16" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B16" t="s">
         <v>4</v>
@@ -1005,8 +1063,8 @@
       <c r="C16" t="s">
         <v>16</v>
       </c>
-      <c r="D16">
-        <v>68546511</v>
+      <c r="D16" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="E16" t="s">
         <v>1</v>

</xml_diff>